<commit_message>
Fixed AI_Summary, refactor project structure and cleanup
</commit_message>
<xml_diff>
--- a/REW/Config.xlsx
+++ b/REW/Config.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29704"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A487B68A-E4E6-4164-9C52-9060ECA151F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{72DE447F-95B0-4AFD-BF05-E336212E390E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Name</t>
   </si>
@@ -48,20 +48,34 @@
     <t>Sector</t>
   </si>
   <si>
-    <t>NrRooms</t>
+    <t>Rooms</t>
   </si>
   <si>
     <t>MinSurface</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>tunaru.alexandra2005@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -84,13 +98,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -403,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -427,7 +444,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>50000</v>
+        <v>70000</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -435,7 +452,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>120000</v>
+        <v>130000</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -462,7 +479,18 @@
         <v>50</v>
       </c>
     </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{1102888F-0DC0-4859-8EA6-85BA49747077}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed max price typing in Scrape_OLX
</commit_message>
<xml_diff>
--- a/REW/Config.xlsx
+++ b/REW/Config.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29704"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{72DE447F-95B0-4AFD-BF05-E336212E390E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -57,14 +56,14 @@
     <t>Email</t>
   </si>
   <si>
-    <t>tunaru.alexandra2005@gmail.com</t>
+    <t>andra.andruta60@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -412,26 +411,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.06640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -439,7 +439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -447,7 +447,7 @@
         <v>70000</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -455,7 +455,7 @@
         <v>130000</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -463,7 +463,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -471,7 +471,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -479,7 +479,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -489,7 +489,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1" xr:uid="{1102888F-0DC0-4859-8EA6-85BA49747077}"/>
+    <hyperlink ref="B7" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed AI_Summary and Send_email from Config
</commit_message>
<xml_diff>
--- a/REW/Config.xlsx
+++ b/REW/Config.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29711"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{300FF799-9B03-45D9-ABBF-EA75DD74FA8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -56,14 +57,14 @@
     <t>Email</t>
   </si>
   <si>
-    <t>andra.andruta60@gmail.com</t>
+    <t>tunaru.alexandra2005@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -411,27 +412,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="10.86328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.06640625" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -439,7 +440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -447,7 +448,7 @@
         <v>70000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -455,7 +456,7 @@
         <v>130000</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -463,7 +464,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -471,7 +472,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -479,7 +480,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" ht="15">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -489,7 +490,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1"/>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed Data extracting for Storia
</commit_message>
<xml_diff>
--- a/REW/Config.xlsx
+++ b/REW/Config.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29711"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{300FF799-9B03-45D9-ABBF-EA75DD74FA8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -57,14 +56,14 @@
     <t>Email</t>
   </si>
   <si>
-    <t>tunaru.alexandra2005@gmail.com</t>
+    <t>andra.andruta60@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -412,27 +411,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.86328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -440,31 +439,31 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
-        <v>70000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>120000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
-        <v>130000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>170000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -472,7 +471,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -480,7 +479,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -490,7 +489,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B7" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed OLX location search
</commit_message>
<xml_diff>
--- a/REW/Config.xlsx
+++ b/REW/Config.xlsx
@@ -411,7 +411,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -444,7 +444,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>120000</v>
+        <v>70000</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
@@ -460,7 +460,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">

</xml_diff>